<commit_message>
Fix alarm filtering and newline formatting
- Filter alarm summary to only include tags with 'alarm' in description
- Reduced from 32 to 13 alarm entries (removed non-alarm status items)
- Fixed newline characters in Excel headers (changed \\n to \n)
- Headers now properly wrap text with actual line breaks
</commit_message>
<xml_diff>
--- a/Alarm_Summary_Output.xlsx
+++ b/Alarm_Summary_Output.xlsx
@@ -433,7 +433,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -482,7 +482,8 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Normal Operating\nConditions</t>
+          <t>Normal Operating
+Conditions</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
@@ -556,13 +557,13 @@
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>B3:0/1</t>
+          <t>B3:3/8</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr"/>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>Fire Eye Faulted Zone 1</t>
+          <t>FE 1 Failure Alarm</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr"/>
@@ -577,13 +578,13 @@
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>B3:0/3</t>
+          <t>B3:3/9</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr"/>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>Fire Eye Faulted Zone 2</t>
+          <t>FE 2 Failure Alarm</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr"/>
@@ -598,13 +599,13 @@
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>B3:0/4</t>
+          <t>B3:3/10</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr"/>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>Fire Detected Zone 2 Fire Eyes. Single Detector Only</t>
+          <t>FE 3 Failure Alarm</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr"/>
@@ -619,13 +620,13 @@
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>B3:0/5</t>
+          <t>B3:3/11</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr"/>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>Fire Detected Zone 1 Fire Eyes. Single Detector Only</t>
+          <t>FE 4 Failure Alarm</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr"/>
@@ -640,13 +641,13 @@
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>B3:0/6</t>
+          <t>B3:3/12</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr"/>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>Plant ESD</t>
+          <t>FE 5 Failure Alarm</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr"/>
@@ -661,13 +662,13 @@
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>B3:0/8</t>
+          <t>B3:3/13</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr"/>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>Fire Eye Failure Warning</t>
+          <t>FE 6 Failure Alarm</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr"/>
@@ -682,13 +683,13 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>B3:0/9</t>
+          <t>B3:3/14</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr"/>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>Strobe Light On</t>
+          <t>FE 7 Failure Alarm</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr"/>
@@ -703,13 +704,13 @@
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>B3:0/10</t>
+          <t>B3:3/15</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr"/>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Strobe Light On</t>
+          <t>FE 8 Failure Alarm</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr"/>
@@ -724,13 +725,13 @@
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>B3:0/12</t>
+          <t>B3:4/6</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr"/>
       <c r="C12" s="2" t="inlineStr">
         <is>
-          <t>Fire System Deluge Valve Open</t>
+          <t>2 Detectors In Alarm Zone 1</t>
         </is>
       </c>
       <c r="D12" s="2" t="inlineStr"/>
@@ -745,13 +746,13 @@
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>B3:0/13</t>
+          <t>B3:4/5</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr"/>
       <c r="C13" s="2" t="inlineStr">
         <is>
-          <t>Strobe Light On</t>
+          <t>2 Detectors In Alarm Zone 2</t>
         </is>
       </c>
       <c r="D13" s="2" t="inlineStr"/>
@@ -766,13 +767,13 @@
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>B3:3/8</t>
+          <t>B3:10/0</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr"/>
       <c r="C14" s="2" t="inlineStr">
         <is>
-          <t>FE 1 Failure Alarm</t>
+          <t>ESD Alarm to Office PLC</t>
         </is>
       </c>
       <c r="D14" s="2" t="inlineStr"/>
@@ -784,405 +785,6 @@
       <c r="J14" s="2" t="inlineStr"/>
       <c r="K14" s="2" t="inlineStr"/>
     </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/9</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="inlineStr"/>
-      <c r="C15" s="2" t="inlineStr">
-        <is>
-          <t>FE 2 Failure Alarm</t>
-        </is>
-      </c>
-      <c r="D15" s="2" t="inlineStr"/>
-      <c r="E15" s="2" t="inlineStr"/>
-      <c r="F15" s="2" t="inlineStr"/>
-      <c r="G15" s="2" t="inlineStr"/>
-      <c r="H15" s="2" t="inlineStr"/>
-      <c r="I15" s="2" t="inlineStr"/>
-      <c r="J15" s="2" t="inlineStr"/>
-      <c r="K15" s="2" t="inlineStr"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/10</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="inlineStr"/>
-      <c r="C16" s="2" t="inlineStr">
-        <is>
-          <t>FE 3 Failure Alarm</t>
-        </is>
-      </c>
-      <c r="D16" s="2" t="inlineStr"/>
-      <c r="E16" s="2" t="inlineStr"/>
-      <c r="F16" s="2" t="inlineStr"/>
-      <c r="G16" s="2" t="inlineStr"/>
-      <c r="H16" s="2" t="inlineStr"/>
-      <c r="I16" s="2" t="inlineStr"/>
-      <c r="J16" s="2" t="inlineStr"/>
-      <c r="K16" s="2" t="inlineStr"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/11</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="inlineStr"/>
-      <c r="C17" s="2" t="inlineStr">
-        <is>
-          <t>FE 4 Failure Alarm</t>
-        </is>
-      </c>
-      <c r="D17" s="2" t="inlineStr"/>
-      <c r="E17" s="2" t="inlineStr"/>
-      <c r="F17" s="2" t="inlineStr"/>
-      <c r="G17" s="2" t="inlineStr"/>
-      <c r="H17" s="2" t="inlineStr"/>
-      <c r="I17" s="2" t="inlineStr"/>
-      <c r="J17" s="2" t="inlineStr"/>
-      <c r="K17" s="2" t="inlineStr"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/12</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="inlineStr"/>
-      <c r="C18" s="2" t="inlineStr">
-        <is>
-          <t>FE 5 Failure Alarm</t>
-        </is>
-      </c>
-      <c r="D18" s="2" t="inlineStr"/>
-      <c r="E18" s="2" t="inlineStr"/>
-      <c r="F18" s="2" t="inlineStr"/>
-      <c r="G18" s="2" t="inlineStr"/>
-      <c r="H18" s="2" t="inlineStr"/>
-      <c r="I18" s="2" t="inlineStr"/>
-      <c r="J18" s="2" t="inlineStr"/>
-      <c r="K18" s="2" t="inlineStr"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/13</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="inlineStr"/>
-      <c r="C19" s="2" t="inlineStr">
-        <is>
-          <t>FE 6 Failure Alarm</t>
-        </is>
-      </c>
-      <c r="D19" s="2" t="inlineStr"/>
-      <c r="E19" s="2" t="inlineStr"/>
-      <c r="F19" s="2" t="inlineStr"/>
-      <c r="G19" s="2" t="inlineStr"/>
-      <c r="H19" s="2" t="inlineStr"/>
-      <c r="I19" s="2" t="inlineStr"/>
-      <c r="J19" s="2" t="inlineStr"/>
-      <c r="K19" s="2" t="inlineStr"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/14</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="inlineStr"/>
-      <c r="C20" s="2" t="inlineStr">
-        <is>
-          <t>FE 7 Failure Alarm</t>
-        </is>
-      </c>
-      <c r="D20" s="2" t="inlineStr"/>
-      <c r="E20" s="2" t="inlineStr"/>
-      <c r="F20" s="2" t="inlineStr"/>
-      <c r="G20" s="2" t="inlineStr"/>
-      <c r="H20" s="2" t="inlineStr"/>
-      <c r="I20" s="2" t="inlineStr"/>
-      <c r="J20" s="2" t="inlineStr"/>
-      <c r="K20" s="2" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/15</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="inlineStr"/>
-      <c r="C21" s="2" t="inlineStr">
-        <is>
-          <t>FE 8 Failure Alarm</t>
-        </is>
-      </c>
-      <c r="D21" s="2" t="inlineStr"/>
-      <c r="E21" s="2" t="inlineStr"/>
-      <c r="F21" s="2" t="inlineStr"/>
-      <c r="G21" s="2" t="inlineStr"/>
-      <c r="H21" s="2" t="inlineStr"/>
-      <c r="I21" s="2" t="inlineStr"/>
-      <c r="J21" s="2" t="inlineStr"/>
-      <c r="K21" s="2" t="inlineStr"/>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/0</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="inlineStr"/>
-      <c r="C22" s="2" t="inlineStr">
-        <is>
-          <t>Fire Eye 1 Fire Detected</t>
-        </is>
-      </c>
-      <c r="D22" s="2" t="inlineStr"/>
-      <c r="E22" s="2" t="inlineStr"/>
-      <c r="F22" s="2" t="inlineStr"/>
-      <c r="G22" s="2" t="inlineStr"/>
-      <c r="H22" s="2" t="inlineStr"/>
-      <c r="I22" s="2" t="inlineStr"/>
-      <c r="J22" s="2" t="inlineStr"/>
-      <c r="K22" s="2" t="inlineStr"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/1</t>
-        </is>
-      </c>
-      <c r="B23" s="2" t="inlineStr"/>
-      <c r="C23" s="2" t="inlineStr">
-        <is>
-          <t>Fire Eye 2 Fire Detected</t>
-        </is>
-      </c>
-      <c r="D23" s="2" t="inlineStr"/>
-      <c r="E23" s="2" t="inlineStr"/>
-      <c r="F23" s="2" t="inlineStr"/>
-      <c r="G23" s="2" t="inlineStr"/>
-      <c r="H23" s="2" t="inlineStr"/>
-      <c r="I23" s="2" t="inlineStr"/>
-      <c r="J23" s="2" t="inlineStr"/>
-      <c r="K23" s="2" t="inlineStr"/>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/2</t>
-        </is>
-      </c>
-      <c r="B24" s="2" t="inlineStr"/>
-      <c r="C24" s="2" t="inlineStr">
-        <is>
-          <t>Fire Eye 3 Fire Detected</t>
-        </is>
-      </c>
-      <c r="D24" s="2" t="inlineStr"/>
-      <c r="E24" s="2" t="inlineStr"/>
-      <c r="F24" s="2" t="inlineStr"/>
-      <c r="G24" s="2" t="inlineStr"/>
-      <c r="H24" s="2" t="inlineStr"/>
-      <c r="I24" s="2" t="inlineStr"/>
-      <c r="J24" s="2" t="inlineStr"/>
-      <c r="K24" s="2" t="inlineStr"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/3</t>
-        </is>
-      </c>
-      <c r="B25" s="2" t="inlineStr"/>
-      <c r="C25" s="2" t="inlineStr">
-        <is>
-          <t>Fire Eye 4 Fire Detected</t>
-        </is>
-      </c>
-      <c r="D25" s="2" t="inlineStr"/>
-      <c r="E25" s="2" t="inlineStr"/>
-      <c r="F25" s="2" t="inlineStr"/>
-      <c r="G25" s="2" t="inlineStr"/>
-      <c r="H25" s="2" t="inlineStr"/>
-      <c r="I25" s="2" t="inlineStr"/>
-      <c r="J25" s="2" t="inlineStr"/>
-      <c r="K25" s="2" t="inlineStr"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/4</t>
-        </is>
-      </c>
-      <c r="B26" s="2" t="inlineStr"/>
-      <c r="C26" s="2" t="inlineStr">
-        <is>
-          <t>Fire Eye 5 Fire Detected</t>
-        </is>
-      </c>
-      <c r="D26" s="2" t="inlineStr"/>
-      <c r="E26" s="2" t="inlineStr"/>
-      <c r="F26" s="2" t="inlineStr"/>
-      <c r="G26" s="2" t="inlineStr"/>
-      <c r="H26" s="2" t="inlineStr"/>
-      <c r="I26" s="2" t="inlineStr"/>
-      <c r="J26" s="2" t="inlineStr"/>
-      <c r="K26" s="2" t="inlineStr"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/5</t>
-        </is>
-      </c>
-      <c r="B27" s="2" t="inlineStr"/>
-      <c r="C27" s="2" t="inlineStr">
-        <is>
-          <t>Fire Eye 6 Fire Detected</t>
-        </is>
-      </c>
-      <c r="D27" s="2" t="inlineStr"/>
-      <c r="E27" s="2" t="inlineStr"/>
-      <c r="F27" s="2" t="inlineStr"/>
-      <c r="G27" s="2" t="inlineStr"/>
-      <c r="H27" s="2" t="inlineStr"/>
-      <c r="I27" s="2" t="inlineStr"/>
-      <c r="J27" s="2" t="inlineStr"/>
-      <c r="K27" s="2" t="inlineStr"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/6</t>
-        </is>
-      </c>
-      <c r="B28" s="2" t="inlineStr"/>
-      <c r="C28" s="2" t="inlineStr">
-        <is>
-          <t>Fire Eye 7 Fire Detected</t>
-        </is>
-      </c>
-      <c r="D28" s="2" t="inlineStr"/>
-      <c r="E28" s="2" t="inlineStr"/>
-      <c r="F28" s="2" t="inlineStr"/>
-      <c r="G28" s="2" t="inlineStr"/>
-      <c r="H28" s="2" t="inlineStr"/>
-      <c r="I28" s="2" t="inlineStr"/>
-      <c r="J28" s="2" t="inlineStr"/>
-      <c r="K28" s="2" t="inlineStr"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="inlineStr">
-        <is>
-          <t>B3:3/7</t>
-        </is>
-      </c>
-      <c r="B29" s="2" t="inlineStr"/>
-      <c r="C29" s="2" t="inlineStr">
-        <is>
-          <t>Fire Eye 8 Fire Detected</t>
-        </is>
-      </c>
-      <c r="D29" s="2" t="inlineStr"/>
-      <c r="E29" s="2" t="inlineStr"/>
-      <c r="F29" s="2" t="inlineStr"/>
-      <c r="G29" s="2" t="inlineStr"/>
-      <c r="H29" s="2" t="inlineStr"/>
-      <c r="I29" s="2" t="inlineStr"/>
-      <c r="J29" s="2" t="inlineStr"/>
-      <c r="K29" s="2" t="inlineStr"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>B3:4/6</t>
-        </is>
-      </c>
-      <c r="B30" s="2" t="inlineStr"/>
-      <c r="C30" s="2" t="inlineStr">
-        <is>
-          <t>2 Detectors In Alarm Zone 1</t>
-        </is>
-      </c>
-      <c r="D30" s="2" t="inlineStr"/>
-      <c r="E30" s="2" t="inlineStr"/>
-      <c r="F30" s="2" t="inlineStr"/>
-      <c r="G30" s="2" t="inlineStr"/>
-      <c r="H30" s="2" t="inlineStr"/>
-      <c r="I30" s="2" t="inlineStr"/>
-      <c r="J30" s="2" t="inlineStr"/>
-      <c r="K30" s="2" t="inlineStr"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>B3:4/5</t>
-        </is>
-      </c>
-      <c r="B31" s="2" t="inlineStr"/>
-      <c r="C31" s="2" t="inlineStr">
-        <is>
-          <t>2 Detectors In Alarm Zone 2</t>
-        </is>
-      </c>
-      <c r="D31" s="2" t="inlineStr"/>
-      <c r="E31" s="2" t="inlineStr"/>
-      <c r="F31" s="2" t="inlineStr"/>
-      <c r="G31" s="2" t="inlineStr"/>
-      <c r="H31" s="2" t="inlineStr"/>
-      <c r="I31" s="2" t="inlineStr"/>
-      <c r="J31" s="2" t="inlineStr"/>
-      <c r="K31" s="2" t="inlineStr"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t>B3:10/0</t>
-        </is>
-      </c>
-      <c r="B32" s="2" t="inlineStr"/>
-      <c r="C32" s="2" t="inlineStr">
-        <is>
-          <t>ESD Alarm to Office PLC</t>
-        </is>
-      </c>
-      <c r="D32" s="2" t="inlineStr"/>
-      <c r="E32" s="2" t="inlineStr"/>
-      <c r="F32" s="2" t="inlineStr"/>
-      <c r="G32" s="2" t="inlineStr"/>
-      <c r="H32" s="2" t="inlineStr"/>
-      <c r="I32" s="2" t="inlineStr"/>
-      <c r="J32" s="2" t="inlineStr"/>
-      <c r="K32" s="2" t="inlineStr"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="inlineStr">
-        <is>
-          <t>O:0/0</t>
-        </is>
-      </c>
-      <c r="B33" s="2" t="inlineStr"/>
-      <c r="C33" s="2" t="inlineStr">
-        <is>
-          <t>Deluge Valve Zone 2 Open</t>
-        </is>
-      </c>
-      <c r="D33" s="2" t="inlineStr"/>
-      <c r="E33" s="2" t="inlineStr"/>
-      <c r="F33" s="2" t="inlineStr"/>
-      <c r="G33" s="2" t="inlineStr"/>
-      <c r="H33" s="2" t="inlineStr"/>
-      <c r="I33" s="2" t="inlineStr"/>
-      <c r="J33" s="2" t="inlineStr"/>
-      <c r="K33" s="2" t="inlineStr"/>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>